<commit_message>
Enhanced UI in FA_all.py with improved layout and styling for file upload and analysis parameters sections. Added new sections for window settings and batch processing, including tooltips for better user guidance. Updated button styles for consistency and visual appeal. Adjusted Flask server to run on localhost.
</commit_message>
<xml_diff>
--- a/saved_data/Hobbit_en.txt in.xlsx
+++ b/saved_data/Hobbit_en.txt in.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -53,18 +53,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,225 +452,214 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>238</v>
+        <v>500</v>
       </c>
       <c r="B2" t="n">
-        <v>1.978280503366497</v>
+        <v>3.069653889284591</v>
       </c>
       <c r="C2" t="n">
-        <v>2.061164532088062</v>
+        <v>3.335148170911226</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>476</v>
+        <v>1000</v>
       </c>
       <c r="B3" t="n">
-        <v>2.879833392374788</v>
+        <v>4.429804532502494</v>
       </c>
       <c r="C3" t="n">
-        <v>3.018737020119576</v>
+        <v>4.518919412959403</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>714</v>
+        <v>1500</v>
       </c>
       <c r="B4" t="n">
-        <v>3.651217171528671</v>
+        <v>5.334960779615662</v>
       </c>
       <c r="C4" t="n">
-        <v>3.773644193942598</v>
+        <v>5.397622850611862</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>952</v>
+        <v>2000</v>
       </c>
       <c r="B5" t="n">
-        <v>4.313319411949202</v>
+        <v>6.145941898393136</v>
       </c>
       <c r="C5" t="n">
-        <v>4.421176987461901</v>
+        <v>6.122856201390911</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1190</v>
+        <v>2500</v>
       </c>
       <c r="B6" t="n">
-        <v>4.905646706107396</v>
+        <v>6.816020514158049</v>
       </c>
       <c r="C6" t="n">
-        <v>4.9990266144144</v>
+        <v>6.751847762248596</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1428</v>
+        <v>3000</v>
       </c>
       <c r="B7" t="n">
-        <v>5.432518536647382</v>
+        <v>7.395939851963604</v>
       </c>
       <c r="C7" t="n">
-        <v>5.526797716373236</v>
+        <v>7.313444990601127</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1666</v>
+        <v>3500</v>
       </c>
       <c r="B8" t="n">
-        <v>5.97636193743872</v>
+        <v>7.940500039650714</v>
       </c>
       <c r="C8" t="n">
-        <v>6.016262822487677</v>
+        <v>7.824559330911549</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1904</v>
+        <v>4000</v>
       </c>
       <c r="B9" t="n">
-        <v>6.525264583395386</v>
+        <v>8.373555978848787</v>
       </c>
       <c r="C9" t="n">
-        <v>6.475160248867392</v>
+        <v>8.29609130789072</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2142</v>
+        <v>4500</v>
       </c>
       <c r="B10" t="n">
-        <v>7.011375522240204</v>
+        <v>8.795707876050505</v>
       </c>
       <c r="C10" t="n">
-        <v>6.908905272132957</v>
+        <v>8.735543653368561</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2380</v>
+        <v>5000</v>
       </c>
       <c r="B11" t="n">
-        <v>7.441237013698237</v>
+        <v>9.198734421718591</v>
       </c>
       <c r="C11" t="n">
-        <v>7.321466321860343</v>
+        <v>9.148335954691776</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2618</v>
+        <v>5500</v>
       </c>
       <c r="B12" t="n">
-        <v>7.882178485202172</v>
+        <v>9.609058089643931</v>
       </c>
       <c r="C12" t="n">
-        <v>7.715856432139184</v>
+        <v>9.538531009233115</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2856</v>
+        <v>6000</v>
       </c>
       <c r="B13" t="n">
-        <v>8.286020597197657</v>
+        <v>9.964032169466703</v>
       </c>
       <c r="C13" t="n">
-        <v>8.094428469631461</v>
+        <v>9.909265450898557</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>3094</v>
+        <v>6500</v>
       </c>
       <c r="B14" t="n">
-        <v>8.649968345954402</v>
+        <v>10.28937092092352</v>
       </c>
       <c r="C14" t="n">
-        <v>8.459062267334536</v>
+        <v>10.2630195234783</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3332</v>
+        <v>7000</v>
       </c>
       <c r="B15" t="n">
-        <v>8.994821277849628</v>
+        <v>10.61427501517862</v>
       </c>
       <c r="C15" t="n">
-        <v>8.811288483900952</v>
+        <v>10.60179375738146</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3570</v>
+        <v>7500</v>
       </c>
       <c r="B16" t="n">
-        <v>9.306320083279036</v>
+        <v>10.89400910350406</v>
       </c>
       <c r="C16" t="n">
-        <v>9.15237355638887</v>
+        <v>10.92722898587394</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3808</v>
+        <v>8000</v>
       </c>
       <c r="B17" t="n">
-        <v>9.572820917600957</v>
+        <v>11.21266361154406</v>
       </c>
       <c r="C17" t="n">
-        <v>9.483379735173685</v>
+        <v>11.24069041066572</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>4046</v>
+        <v>8500</v>
       </c>
       <c r="B18" t="n">
-        <v>9.801711104781528</v>
+        <v>11.48195363740862</v>
       </c>
       <c r="C18" t="n">
-        <v>9.80520860290226</v>
+        <v>11.54332804302194</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>4284</v>
+        <v>9000</v>
       </c>
       <c r="B19" t="n">
-        <v>10.00798650326697</v>
+        <v>11.76149241736466</v>
       </c>
       <c r="C19" t="n">
-        <v>10.118633320533</v>
+        <v>11.8361211481576</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>4522</v>
+        <v>9500</v>
       </c>
       <c r="B20" t="n">
-        <v>10.189299537241</v>
+        <v>12.00139562254284</v>
       </c>
       <c r="C20" t="n">
-        <v>10.42432298137055</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>4760</v>
-      </c>
-      <c r="B21" t="n">
-        <v>10.36177458307811</v>
-      </c>
-      <c r="C21" t="n">
-        <v>10.72286131615535</v>
+        <v>12.11991157349273</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>